<commit_message>
[FEATURE]Dual,DDS,CUSTOM_WAVE and optimized BSRAM.
Optimized:
	+ Reduce UART RX FIFO to 64 Bytes.
	+ Reduce I2C BUFFER to 64 Bytes.
	+ Remove PLL_INIT for PLL IP cores that do not use variable
	  frequency.
</commit_message>
<xml_diff>
--- a/doc/引脚对照表-自制板子.xlsx
+++ b/doc/引脚对照表-自制板子.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GOWIN\FPGA2025\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80EF8F-7817-4A1A-9D24-588BA87168E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8C5F37-05FA-41AE-B34C-3183EC31714A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
   <si>
     <t>PWM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,6 +122,87 @@
   </si>
   <si>
     <t>OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i2c_scl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i2c_sda</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INOUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dc_signal_in[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dc_signal_in[1]</t>
+  </si>
+  <si>
+    <t>dc_signal_in[2]</t>
+  </si>
+  <si>
+    <t>dc_signal_in[3]</t>
+  </si>
+  <si>
+    <t>dc_signal_in[4]</t>
+  </si>
+  <si>
+    <t>dc_signal_in[5]</t>
+  </si>
+  <si>
+    <t>dc_signal_in[6]</t>
+  </si>
+  <si>
+    <t>dc_signal_in[7]</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>N14</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>N16</t>
+  </si>
+  <si>
+    <t>N15</t>
+  </si>
+  <si>
+    <t>M18</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>IN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -632,9 +713,195 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>